<commit_message>
Inclusión de una imagen extra en solicitud gráfica
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado08/guion01/CN_08_01_CO_REC210_SolicitudGrafica.xlsx
+++ b/fuentes/contenidos/grado08/guion01/CN_08_01_CO_REC210_SolicitudGrafica.xlsx
@@ -5,7 +5,7 @@
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documentos E\Aula Planeta\Edición\Amanda Varela\CN_08_01_CO\Procesar Jose\Procesado\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Miguel\Documents\GitHub\CienciasNaturales\fuentes\contenidos\grado08\guion01\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="hX79YNGfHMUCcosWMoH0GQuhNo2gkebFrfW3do2TOcvwqaujU9m0uwOL5UkRtWEspAy/ISD2JB8+jf057W9mVA==" workbookSaltValue="uRz/CDpmZ5ecKheoN1C0Jw==" workbookSpinCount="100000" lockStructure="1"/>
@@ -21,12 +21,12 @@
     <definedName name="Formato">'Solicitud gráfica'!$L$2:$L$3</definedName>
     <definedName name="Ubicación">'Solicitud gráfica'!$M$2:$M$6</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="215">
   <si>
     <t>Fecha:</t>
   </si>
@@ -669,6 +669,9 @@
   </si>
   <si>
     <t>Cambiar "Inflammation" por "Inflamación", cambiar "Brain" por "Cerebro" en ambos casos, cambiar "Scull" por "Cráneo", unir y cambiar "Dura, Arachnoid y Pia mater" por "Meninges". Es decir, queda una sola capa, con un solo color, llamada meninges. Quitar los demás textos. Quitar la imagen circular inferior izquierda.</t>
+  </si>
+  <si>
+    <t>Hombre con dolor de cabeza</t>
   </si>
 </sst>
 </file>
@@ -2545,8 +2548,8 @@
   <dimension ref="A1:P108"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="140" workbookViewId="0">
-      <pane ySplit="9" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B24" sqref="B24"/>
+      <pane ySplit="9" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J29" sqref="J29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -3640,35 +3643,43 @@
       </c>
       <c r="K28" s="64"/>
     </row>
-    <row r="29" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" s="11" customFormat="1" ht="27" x14ac:dyDescent="0.25">
       <c r="A29" s="12" t="str">
         <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="B29" s="62"/>
+        <v>IMG20</v>
+      </c>
+      <c r="B29" s="62">
+        <v>183922637</v>
+      </c>
       <c r="C29" s="20" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="D29" s="63"/>
-      <c r="E29" s="63"/>
+        <v>Recurso F6</v>
+      </c>
+      <c r="D29" s="63" t="s">
+        <v>197</v>
+      </c>
+      <c r="E29" s="63" t="s">
+        <v>155</v>
+      </c>
       <c r="F29" s="13" t="str">
-        <f t="shared" si="4"/>
-        <v/>
+        <f t="shared" ca="1" si="4"/>
+        <v>CN_08_01_CO_REC210_IMG20n.jpg</v>
       </c>
       <c r="G29" s="13" t="str">
         <f ca="1">IF($F29&lt;&gt;"",IF($G$4="Recurso",VLOOKUP($E29,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),5),5,FALSE),'Definición técnica de imagenes'!$F$16),"")</f>
-        <v/>
+        <v>320 x 480 px</v>
       </c>
       <c r="H29" s="13" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v/>
+        <v>CN_08_01_CO_REC210_IMG20a.jpg</v>
       </c>
       <c r="I29" s="13" t="str">
         <f ca="1">IF(OR($B29&lt;&gt;"",$J29&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E29,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E29,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
-        <v/>
-      </c>
-      <c r="J29" s="64"/>
+        <v>800 x 458 px</v>
+      </c>
+      <c r="J29" s="64" t="s">
+        <v>214</v>
+      </c>
       <c r="K29" s="64"/>
     </row>
     <row r="30" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.25">

</xml_diff>